<commit_message>
Added hours to time card - M.D.
</commit_message>
<xml_diff>
--- a/Iteration-1/time_cards.xlsx
+++ b/Iteration-1/time_cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Software Engineering 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Desktop/Code/CSI-3471/Project/C.A.R./Iteration-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1AE7E24-3728-4D5E-8ADD-6BA5F9BE96B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396A33FF-429B-F143-9F6B-872A14043D9E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{B62098E1-3187-41F4-98CC-20B71604981B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14020" xr2:uid="{B62098E1-3187-41F4-98CC-20B71604981B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>8h 14m</t>
+  </si>
+  <si>
+    <t>8h 15m</t>
   </si>
 </sst>
 </file>
@@ -423,15 +426,15 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="18.42578125" customWidth="1"/>
+    <col min="1" max="2" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,17 +442,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -457,17 +463,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Cleaned up iteration 1 folder Added my time spent as of right now to time_cards
</commit_message>
<xml_diff>
--- a/Iteration-1/time_cards.xlsx
+++ b/Iteration-1/time_cards.xlsx
@@ -1,36 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Desktop/Code/CSI-3471/Project/C.A.R./Iteration-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewCase/C.A.R./Iteration-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396A33FF-429B-F143-9F6B-872A14043D9E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDCD0EA-9228-524D-9B4A-23768AC4AF8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14020" xr2:uid="{B62098E1-3187-41F4-98CC-20B71604981B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14020" xr2:uid="{B62098E1-3187-41F4-98CC-20B71604981B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -63,6 +58,9 @@
   </si>
   <si>
     <t>8h 15m</t>
+  </si>
+  <si>
+    <t>8h 30m</t>
   </si>
 </sst>
 </file>
@@ -446,6 +444,9 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">

</xml_diff>